<commit_message>
tests(urban_district_upscaling): update sink tests
</commit_message>
<xml_diff>
--- a/program_files/urban_district_upscaling/standard_parameters.xlsx
+++ b/program_files/urban_district_upscaling/standard_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/program_files/urban_district_upscaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA0937D-9E06-5D44-99C2-1ED6D30299D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF37AA1-8416-EC44-B3A2-04F3B9F8175F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" activeTab="3" xr2:uid="{E7C0A991-ABA2-4650-8848-5C73E0926BAC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" activeTab="2" xr2:uid="{E7C0A991-ABA2-4650-8848-5C73E0926BAC}"/>
   </bookViews>
   <sheets>
     <sheet name="energysystem" sheetId="1" r:id="rId1"/>
@@ -255,18 +255,6 @@
     <t>efh</t>
   </si>
   <si>
-    <t>RES_SFB_electricity_sink</t>
-  </si>
-  <si>
-    <t>RES_SFB_heat_sink</t>
-  </si>
-  <si>
-    <t>RES_MFB_electricity_sink</t>
-  </si>
-  <si>
-    <t>RES_MFB_heat_sink</t>
-  </si>
-  <si>
     <t>mfh</t>
   </si>
   <si>
@@ -1009,6 +997,18 @@
   </si>
   <si>
     <t>1 unit(s)</t>
+  </si>
+  <si>
+    <t>SFB_electricity_sink</t>
+  </si>
+  <si>
+    <t>SFB_heat_sink</t>
+  </si>
+  <si>
+    <t>MFB_electricity_sink</t>
+  </si>
+  <si>
+    <t>MFB_heat_sink</t>
   </si>
 </sst>
 </file>
@@ -1178,7 +1178,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
@@ -1211,6 +1211,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1608,16 +1609,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="H1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
@@ -1639,16 +1640,16 @@
         <v>8760</v>
       </c>
       <c r="E3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="H3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -1674,21 +1675,21 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B2" s="14">
         <v>1.3</v>
@@ -3214,7 +3215,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B110" s="16">
         <v>0.35</v>
@@ -3229,7 +3230,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B111" s="16">
         <v>0.21</v>
@@ -3243,7 +3244,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B112" s="16">
         <v>9.35</v>
@@ -3257,7 +3258,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B113" s="16">
         <v>7.14</v>
@@ -3271,7 +3272,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B114" s="16">
         <v>286</v>
@@ -3285,7 +3286,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B115" s="16">
         <v>286</v>
@@ -3344,18 +3345,18 @@
         <v>11</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>13</v>
@@ -3387,7 +3388,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>13</v>
@@ -3451,7 +3452,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>13</v>
@@ -3483,7 +3484,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>13</v>
@@ -3739,7 +3740,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>13</v>
@@ -3771,7 +3772,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>13</v>
@@ -3803,7 +3804,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>13</v>
@@ -3835,7 +3836,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>13</v>
@@ -3867,7 +3868,7 @@
     </row>
     <row r="18" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="15" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>13</v>
@@ -3899,7 +3900,7 @@
     </row>
     <row r="19" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>13</v>
@@ -3931,7 +3932,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="8" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>13</v>
@@ -3963,7 +3964,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>13</v>
@@ -3995,7 +3996,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>13</v>
@@ -4027,7 +4028,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" s="21" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>13</v>
@@ -4059,7 +4060,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" s="21" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>13</v>
@@ -4091,7 +4092,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25" s="21" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>13</v>
@@ -4123,7 +4124,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A26" s="21" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>13</v>
@@ -4155,7 +4156,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" s="21" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B27" s="21" t="s">
         <v>13</v>
@@ -4187,7 +4188,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A28" s="21" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B28" s="21" t="s">
         <v>13</v>
@@ -4219,7 +4220,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A29" s="21" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B29" s="21" t="s">
         <v>13</v>
@@ -4251,7 +4252,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A30" s="21" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B30" s="21" t="s">
         <v>13</v>
@@ -4283,7 +4284,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A31" s="21" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B31" s="21" t="s">
         <v>13</v>
@@ -4329,8 +4330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{466B86C4-4C4F-403F-9786-83A2FF294476}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -4370,76 +4371,76 @@
         <v>28</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A2" s="11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="11">
-        <v>1</v>
-      </c>
-      <c r="D2" s="11">
-        <v>1</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="C2" s="28">
+        <v>1</v>
+      </c>
+      <c r="D2" s="28">
+        <v>1</v>
+      </c>
+      <c r="E2" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="11">
-        <v>0</v>
-      </c>
-      <c r="G2" s="11">
-        <v>0</v>
-      </c>
-      <c r="H2" s="11">
+      <c r="F2" s="28">
+        <v>0</v>
+      </c>
+      <c r="G2" s="28">
+        <v>0</v>
+      </c>
+      <c r="H2" s="28">
         <v>3</v>
       </c>
-      <c r="I2" s="11">
-        <v>1</v>
-      </c>
-      <c r="J2" s="7">
+      <c r="I2" s="28">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4">
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="11">
-        <v>1</v>
-      </c>
-      <c r="D3" s="11">
-        <v>1</v>
-      </c>
-      <c r="E3" s="11" t="s">
+      <c r="C3" s="28">
+        <v>1</v>
+      </c>
+      <c r="D3" s="28">
+        <v>1</v>
+      </c>
+      <c r="E3" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="11">
-        <v>0</v>
-      </c>
-      <c r="G3" s="11">
-        <v>0</v>
-      </c>
-      <c r="H3" s="11">
+      <c r="F3" s="28">
+        <v>0</v>
+      </c>
+      <c r="G3" s="28">
+        <v>0</v>
+      </c>
+      <c r="H3" s="28">
         <v>3</v>
       </c>
-      <c r="I3" s="11">
-        <v>1</v>
-      </c>
-      <c r="J3" s="7">
+      <c r="I3" s="28">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4">
         <v>0.9</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="11" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>13</v>
@@ -4471,7 +4472,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="11" t="s">
-        <v>34</v>
+        <v>282</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>13</v>
@@ -4503,7 +4504,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="11" t="s">
-        <v>35</v>
+        <v>283</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>13</v>
@@ -4535,7 +4536,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>36</v>
+        <v>284</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>13</v>
@@ -4547,7 +4548,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F7" s="11">
         <v>0</v>
@@ -4565,75 +4566,75 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A8" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="11" t="s">
+    <row r="8" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="11">
-        <v>1</v>
-      </c>
-      <c r="D8" s="11">
-        <v>1</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="11">
-        <v>0</v>
-      </c>
-      <c r="G8" s="11">
-        <v>0</v>
-      </c>
-      <c r="H8" s="11">
+      <c r="C8" s="28">
+        <v>1</v>
+      </c>
+      <c r="D8" s="28">
+        <v>1</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="28">
+        <v>0</v>
+      </c>
+      <c r="G8" s="28">
+        <v>0</v>
+      </c>
+      <c r="H8" s="28">
         <v>3</v>
       </c>
-      <c r="I8" s="11">
-        <v>1</v>
-      </c>
-      <c r="J8" s="7">
+      <c r="I8" s="28">
+        <v>1</v>
+      </c>
+      <c r="J8" s="4">
         <f>AVERAGE(J9:J18)</f>
         <v>0.88679999999999981</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A9" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="11" t="s">
+    <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="11">
-        <v>1</v>
-      </c>
-      <c r="D9" s="11">
-        <v>1</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="11">
-        <v>0</v>
-      </c>
-      <c r="G9" s="11">
-        <v>0</v>
-      </c>
-      <c r="H9" s="11">
+      <c r="C9" s="28">
+        <v>1</v>
+      </c>
+      <c r="D9" s="28">
+        <v>1</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="28">
+        <v>0</v>
+      </c>
+      <c r="G9" s="28">
+        <v>0</v>
+      </c>
+      <c r="H9" s="28">
         <v>3</v>
       </c>
-      <c r="I9" s="11">
-        <v>1</v>
-      </c>
-      <c r="J9" s="7">
+      <c r="I9" s="28">
+        <v>1</v>
+      </c>
+      <c r="J9" s="4">
         <f>AVERAGE(J10:J19)</f>
         <v>0.8879999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="11" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>13</v>
@@ -4645,7 +4646,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F10" s="11">
         <v>0</v>
@@ -4665,7 +4666,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>13</v>
@@ -4677,7 +4678,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F11" s="11">
         <v>0</v>
@@ -4697,7 +4698,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>13</v>
@@ -4709,7 +4710,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F12" s="11">
         <v>0</v>
@@ -4729,7 +4730,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>13</v>
@@ -4741,7 +4742,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F13" s="11">
         <v>0</v>
@@ -4761,7 +4762,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>13</v>
@@ -4773,7 +4774,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="F14" s="11">
         <v>0</v>
@@ -4793,7 +4794,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>13</v>
@@ -4805,7 +4806,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F15" s="11">
         <v>0</v>
@@ -4825,7 +4826,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>13</v>
@@ -4837,7 +4838,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F16" s="11">
         <v>0</v>
@@ -4857,7 +4858,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>13</v>
@@ -4869,7 +4870,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="F17" s="11">
         <v>0</v>
@@ -4889,7 +4890,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>13</v>
@@ -4901,7 +4902,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F18" s="11">
         <v>0</v>
@@ -4921,7 +4922,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>13</v>
@@ -4933,7 +4934,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F19" s="11">
         <v>0</v>
@@ -4953,7 +4954,7 @@
     </row>
     <row r="20" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A20" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>13</v>
@@ -4965,7 +4966,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F20" s="11">
         <v>0</v>
@@ -4985,7 +4986,7 @@
     </row>
     <row r="21" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>13</v>
@@ -4997,7 +4998,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F21" s="11">
         <v>0</v>
@@ -5017,7 +5018,7 @@
     </row>
     <row r="22" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A22" s="11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>13</v>
@@ -5029,7 +5030,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F22" s="11">
         <v>0</v>
@@ -5049,7 +5050,7 @@
     </row>
     <row r="23" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A23" s="11" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>13</v>
@@ -5061,7 +5062,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F23" s="11">
         <v>0</v>
@@ -5081,7 +5082,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" s="11" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>13</v>
@@ -5093,7 +5094,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F24" s="11">
         <v>0</v>
@@ -5113,7 +5114,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25" s="11" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>13</v>
@@ -5125,7 +5126,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F25" s="11">
         <v>0</v>
@@ -5145,7 +5146,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A26" s="11" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>13</v>
@@ -5157,7 +5158,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F26" s="11">
         <v>0</v>
@@ -5177,7 +5178,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" s="11" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>13</v>
@@ -5189,7 +5190,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F27" s="11">
         <v>0</v>
@@ -5209,7 +5210,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A28" s="11" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>13</v>
@@ -5221,7 +5222,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F28" s="11">
         <v>0</v>
@@ -5241,7 +5242,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A29" s="11" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>13</v>
@@ -5253,7 +5254,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F29" s="11">
         <v>0</v>
@@ -5273,7 +5274,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A30" s="11" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>13</v>
@@ -5285,7 +5286,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F30" s="11">
         <v>0</v>
@@ -5305,7 +5306,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A31" s="11" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>13</v>
@@ -5317,7 +5318,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F31" s="11">
         <v>0</v>
@@ -5346,7 +5347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE5AA59-F323-4C10-A5B0-98A99D49A877}">
   <dimension ref="A1:Y109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5365,84 +5366,84 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="K1" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="M1" s="7" t="s">
+      <c r="O1" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q1" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="N1" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q1" s="12" t="s">
+      <c r="R1" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="S1" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="R1" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>137</v>
-      </c>
       <c r="T1" s="12" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="U1" s="12" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="V1" s="10" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="W1" s="10" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="X1" s="10" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="Y1" s="10" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B2" s="9">
         <v>247</v>
@@ -13785,140 +13786,140 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G1" t="s">
+        <v>266</v>
+      </c>
+      <c r="H1" t="s">
+        <v>267</v>
+      </c>
+      <c r="I1" t="s">
+        <v>268</v>
+      </c>
+      <c r="J1" t="s">
+        <v>269</v>
+      </c>
+      <c r="K1" t="s">
+        <v>270</v>
+      </c>
+      <c r="L1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M1" t="s">
+        <v>130</v>
+      </c>
+      <c r="N1" t="s">
+        <v>131</v>
+      </c>
+      <c r="O1" t="s">
         <v>132</v>
       </c>
-      <c r="B1" t="s">
-        <v>283</v>
-      </c>
-      <c r="C1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E1" t="s">
-        <v>277</v>
-      </c>
-      <c r="F1" t="s">
-        <v>281</v>
-      </c>
-      <c r="G1" t="s">
-        <v>270</v>
-      </c>
-      <c r="H1" t="s">
-        <v>271</v>
-      </c>
-      <c r="I1" t="s">
-        <v>272</v>
-      </c>
-      <c r="J1" t="s">
-        <v>273</v>
-      </c>
-      <c r="K1" t="s">
-        <v>274</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>133</v>
       </c>
-      <c r="M1" t="s">
-        <v>134</v>
-      </c>
-      <c r="N1" t="s">
-        <v>135</v>
-      </c>
-      <c r="O1" t="s">
-        <v>136</v>
-      </c>
-      <c r="P1" t="s">
-        <v>137</v>
-      </c>
       <c r="Q1" s="11" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="R1" s="11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="S1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="T1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="U1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="V1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="G2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="H2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="I2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="J2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="K2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="L2" s="27" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="M2" s="27" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="N2" s="27" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="O2" s="27" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="P2" s="27" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="Q2" s="27" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="R2" s="27" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="S2" s="27" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="T2" s="27" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="U2" s="27" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="V2" s="27" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B3" s="9">
         <v>2300</v>
@@ -13984,7 +13985,7 @@
         <v>115</v>
       </c>
       <c r="V3" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -14029,101 +14030,101 @@
         <v>23</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="J1" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="K1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="N1" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>67</v>
-      </c>
       <c r="R1" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="S1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="W1" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AD1" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AE1" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="AB1" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="AC1" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="AD1" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="AE1" s="7" t="s">
-        <v>150</v>
-      </c>
       <c r="AF1" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B3" s="7">
         <v>1</v>
@@ -14132,7 +14133,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E3" s="7">
         <v>0</v>
@@ -14153,16 +14154,16 @@
         <v>0</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="O3" s="7">
         <v>0.18</v>
@@ -14221,7 +14222,7 @@
     </row>
     <row r="4" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
@@ -14230,7 +14231,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E4" s="26">
         <v>0</v>
@@ -14320,7 +14321,7 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A5" s="21" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B5" s="21">
         <v>1</v>
@@ -14329,7 +14330,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E5" s="21">
         <v>0</v>
@@ -14477,138 +14478,138 @@
         <v>8</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="J1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G1" s="7" t="s">
+      <c r="O1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="R1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="T1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="T1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="Z1" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="AB1" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC1" s="7" t="s">
-        <v>102</v>
-      </c>
       <c r="AD1" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="AH1" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="AE1" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="AF1" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="AG1" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="AH1" s="7" t="s">
-        <v>155</v>
-      </c>
       <c r="AI1" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="AM1" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="AJ1" s="7" t="s">
+      <c r="AN1" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="AK1" s="7" t="s">
+      <c r="AO1" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="AL1" s="7" t="s">
+      <c r="AP1" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="AM1" s="7" t="s">
+      <c r="AQ1" s="7" t="s">
         <v>200</v>
-      </c>
-      <c r="AN1" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="AO1" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="AP1" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="AQ1" s="7" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B2" s="7">
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D2" s="7">
         <v>0.375</v>
@@ -14733,13 +14734,13 @@
     </row>
     <row r="3" spans="1:43" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B3" s="8">
         <v>1</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D3" s="8">
         <v>0.39</v>
@@ -14864,13 +14865,13 @@
     </row>
     <row r="4" spans="1:43" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B4" s="8">
         <v>1</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D4" s="8">
         <v>0.92</v>
@@ -14995,13 +14996,13 @@
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B5" s="7">
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
@@ -15052,10 +15053,10 @@
         <v>0</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="V5" s="7">
         <v>60</v>
@@ -15126,13 +15127,13 @@
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D6" s="7">
         <v>1</v>
@@ -15183,10 +15184,10 @@
         <v>0</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="V6" s="7">
         <v>60</v>
@@ -15257,13 +15258,13 @@
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.15">
       <c r="A7" s="8" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B7" s="7">
         <v>1</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D7" s="7">
         <v>1</v>
@@ -15314,10 +15315,10 @@
         <v>0</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="U7" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="V7" s="7">
         <v>60</v>
@@ -15388,13 +15389,13 @@
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.15">
       <c r="A8" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B8" s="7">
         <v>1</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
@@ -15445,10 +15446,10 @@
         <v>0</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="U8" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="V8" s="7">
         <v>60</v>
@@ -15519,13 +15520,13 @@
     </row>
     <row r="9" spans="1:43" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B9" s="8">
         <v>1</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D9" s="11">
         <v>1</v>
@@ -15650,13 +15651,13 @@
     </row>
     <row r="10" spans="1:43" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A10" s="15" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B10" s="15">
         <v>1</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D10" s="22">
         <v>0.5</v>
@@ -15781,13 +15782,13 @@
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.15">
       <c r="A11" s="8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B11" s="7">
         <v>1</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D11" s="11">
         <v>0.78500000000000003</v>
@@ -15912,13 +15913,13 @@
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.15">
       <c r="A12" s="8" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B12" s="7">
         <v>1</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D12" s="11">
         <v>0.83</v>
@@ -16043,13 +16044,13 @@
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.15">
       <c r="A13" s="8" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B13" s="7">
         <v>1</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D13" s="11">
         <v>0.4</v>
@@ -16174,13 +16175,13 @@
     </row>
     <row r="14" spans="1:43" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="8" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B14" s="8">
         <v>1</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D14" s="11">
         <v>0.98</v>
@@ -16305,13 +16306,13 @@
     </row>
     <row r="15" spans="1:43" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A15" s="8" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B15" s="8">
         <v>1</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D15" s="8">
         <v>0.98</v>
@@ -16436,13 +16437,13 @@
     </row>
     <row r="16" spans="1:43" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A16" s="8" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B16" s="8">
         <v>1</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D16" s="8">
         <v>0.98</v>
@@ -16567,13 +16568,13 @@
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B17" s="7">
         <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D17" s="7">
         <v>0.92</v>
@@ -16698,13 +16699,13 @@
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.15">
       <c r="A18" s="24" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B18" s="24">
         <v>1</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D18" s="21">
         <v>1</v>
@@ -16755,10 +16756,10 @@
         <v>0</v>
       </c>
       <c r="T18" s="21" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="U18" s="21" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="V18" s="21">
         <v>60</v>
@@ -16829,13 +16830,13 @@
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.15">
       <c r="A19" s="24" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B19" s="24">
         <v>1</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D19" s="21">
         <v>0.375</v>
@@ -16960,13 +16961,13 @@
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.15">
       <c r="A20" s="24" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B20" s="24">
         <v>1</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D20" s="21">
         <v>0.375</v>
@@ -17091,13 +17092,13 @@
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.15">
       <c r="A21" s="24" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B21" s="24">
         <v>1</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D21" s="21">
         <v>0.92</v>
@@ -17222,13 +17223,13 @@
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.15">
       <c r="A22" s="24" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B22" s="24">
         <v>1</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D22" s="21">
         <v>0.92</v>
@@ -17353,13 +17354,13 @@
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.15">
       <c r="A23" s="24" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B23" s="24">
         <v>1</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D23" s="21">
         <v>0.92</v>
@@ -17484,7 +17485,7 @@
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.15">
       <c r="D31" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -17525,90 +17526,90 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" t="s">
+        <v>243</v>
+      </c>
+      <c r="L1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M1" t="s">
+        <v>106</v>
+      </c>
+      <c r="N1" t="s">
+        <v>107</v>
+      </c>
+      <c r="O1" t="s">
         <v>108</v>
       </c>
-      <c r="D1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K1" t="s">
-        <v>247</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>109</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>110</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>111</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>112</v>
       </c>
-      <c r="P1" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>114</v>
-      </c>
-      <c r="R1" t="s">
-        <v>115</v>
-      </c>
-      <c r="S1" t="s">
-        <v>116</v>
-      </c>
       <c r="T1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="U1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="V1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="W1" t="s">
+        <v>87</v>
+      </c>
+      <c r="X1" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y1" t="s">
         <v>91</v>
       </c>
-      <c r="X1" t="s">
-        <v>156</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>95</v>
-      </c>
       <c r="Z1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="AA1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B2" s="12">
         <v>1</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D2" s="12">
         <v>0</v>
@@ -17685,13 +17686,13 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D3" s="12">
         <v>0</v>
@@ -17768,13 +17769,13 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D4" s="12">
         <v>0</v>
@@ -17851,13 +17852,13 @@
     </row>
     <row r="5" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D5" s="12">
         <v>0</v>
@@ -17934,13 +17935,13 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B6" s="12">
         <v>1</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D6" s="12">
         <v>0</v>
@@ -18018,13 +18019,13 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B7" s="12">
         <v>1</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D7" s="12">
         <v>0</v>
@@ -18121,7 +18122,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -18130,45 +18131,45 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" t="s">
         <v>76</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>77</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" t="s">
         <v>78</v>
       </c>
-      <c r="G1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J1" t="s">
-        <v>81</v>
-      </c>
-      <c r="K1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M1" t="s">
-        <v>82</v>
-      </c>
       <c r="N1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="O1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -18177,7 +18178,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E2" s="9">
         <v>1</v>
@@ -18215,7 +18216,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="18" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>13</v>
@@ -18224,7 +18225,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E3" s="18">
         <v>1</v>
@@ -18262,7 +18263,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -18271,7 +18272,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E4" s="9">
         <v>1</v>
@@ -18309,7 +18310,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -18318,7 +18319,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E5" s="9">
         <v>1</v>
@@ -18356,7 +18357,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -18365,7 +18366,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E6" s="9">
         <v>1</v>
@@ -18403,7 +18404,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -18412,7 +18413,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E7" s="9">
         <v>1</v>
@@ -18450,7 +18451,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>13</v>
@@ -18459,7 +18460,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E8" s="18">
         <v>0.9</v>
@@ -18497,7 +18498,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>13</v>
@@ -18506,7 +18507,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E9" s="12">
         <v>1</v>
@@ -18544,7 +18545,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>13</v>
@@ -18553,7 +18554,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E10" s="12">
         <v>1</v>

</xml_diff>

<commit_message>
code(urban_district_upscaling): update US Tool
</commit_message>
<xml_diff>
--- a/program_files/urban_district_upscaling/standard_parameters.xlsx
+++ b/program_files/urban_district_upscaling/standard_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregor/Desktop/Arbeit/Git/SESMG/program_files/urban_district_upscaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA1FBC3-C39F-0649-A993-2742A8D0851E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DFAB51-CD91-4949-B855-17D49705C8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18940" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
   <sheets>
     <sheet name="energysystem" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,8 @@
     <sheet name="5_storages" sheetId="8" r:id="rId8"/>
     <sheet name="6_links" sheetId="9" r:id="rId9"/>
     <sheet name="7_insulation" sheetId="10" r:id="rId10"/>
-    <sheet name="8_pipe_types" sheetId="11" r:id="rId11"/>
-    <sheet name="8_1_other" sheetId="12" r:id="rId12"/>
+    <sheet name="8_pipe_types" sheetId="12" r:id="rId11"/>
+    <sheet name="8_1_other" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -871,6 +871,30 @@
     <t>periodical constraint costs flat</t>
   </si>
   <si>
+    <t>building_oilheating_transformer</t>
+  </si>
+  <si>
+    <t>building_res_oil_bus</t>
+  </si>
+  <si>
+    <t>building_com_oil_bus</t>
+  </si>
+  <si>
+    <t>building_ind_oil_bus</t>
+  </si>
+  <si>
+    <t>SFB_electricity_sink</t>
+  </si>
+  <si>
+    <t>SFB_heat_sink</t>
+  </si>
+  <si>
+    <t>MFB_electricity_sink</t>
+  </si>
+  <si>
+    <t>MFB_heat_sink</t>
+  </si>
+  <si>
     <t>label_3</t>
   </si>
   <si>
@@ -901,9 +925,21 @@
     <t>periodical_constraint_costs</t>
   </si>
   <si>
+    <t>anergy_or_exergy</t>
+  </si>
+  <si>
+    <t>distribution_pipe</t>
+  </si>
+  <si>
+    <t>building_pipe</t>
+  </si>
+  <si>
     <t>Diameter-1000</t>
   </si>
   <si>
+    <t>exergy</t>
+  </si>
+  <si>
     <t>Diameter-50</t>
   </si>
   <si>
@@ -925,16 +961,7 @@
     <t>Diameter65L</t>
   </si>
   <si>
-    <t>anergy_or_exergy</t>
-  </si>
-  <si>
-    <t>exergy</t>
-  </si>
-  <si>
-    <t>distribution_pipe</t>
-  </si>
-  <si>
-    <t>building_pipe</t>
+    <t>anergy</t>
   </si>
   <si>
     <t>label</t>
@@ -953,33 +980,6 @@
   </si>
   <si>
     <t>anergy_heat_pump</t>
-  </si>
-  <si>
-    <t>anergy</t>
-  </si>
-  <si>
-    <t>SFB_electricity_sink</t>
-  </si>
-  <si>
-    <t>SFB_heat_sink</t>
-  </si>
-  <si>
-    <t>MFB_electricity_sink</t>
-  </si>
-  <si>
-    <t>MFB_heat_sink</t>
-  </si>
-  <si>
-    <t>building_res_oil_bus</t>
-  </si>
-  <si>
-    <t>building_com_oil_bus</t>
-  </si>
-  <si>
-    <t>building_ind_oil_bus</t>
-  </si>
-  <si>
-    <t>building_oilheating_transformer</t>
   </si>
 </sst>
 </file>
@@ -1004,17 +1004,19 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1067,7 +1069,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1075,9 +1077,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1480,7 +1483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9349B1DA-DD91-4E08-AB6A-4F16A6735056}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -3182,7 +3185,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:D116">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3191,11 +3194,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29FAF5D4-E73D-0B41-A5EE-606E05C3A7C4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEE9DEA-E38F-C741-B378-A7CB5600BE5E}">
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3208,750 +3211,750 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="K1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="D1" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="N1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6">
+      <c r="B2" s="7">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7">
         <v>57.408200000000001</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="7">
         <v>410770</v>
       </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6">
-        <v>0</v>
-      </c>
-      <c r="I2" s="6">
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0</v>
+      </c>
+      <c r="I2" s="7">
         <v>5046</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="7">
         <v>57</v>
       </c>
-      <c r="K2" s="6">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
-        <v>293</v>
-      </c>
-      <c r="M2" s="6">
-        <v>1</v>
-      </c>
-      <c r="N2" s="6">
+      <c r="K2" s="7">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="M2" s="7">
+        <v>1</v>
+      </c>
+      <c r="N2" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="A3" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
         <v>23.674199999999999</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="7">
         <v>26112</v>
       </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0</v>
-      </c>
-      <c r="I3" s="6">
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
         <v>611</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="7">
         <v>24</v>
       </c>
-      <c r="K3" s="6">
-        <v>0</v>
-      </c>
-      <c r="L3" t="s">
-        <v>293</v>
-      </c>
-      <c r="M3" s="6">
-        <v>1</v>
-      </c>
-      <c r="N3" s="6">
+      <c r="K3" s="7">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="M3" s="7">
+        <v>1</v>
+      </c>
+      <c r="N3" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
+      <c r="A4" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
         <v>39.284799999999997</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="7">
         <v>8220</v>
       </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7">
         <v>1174</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="7">
         <v>39</v>
       </c>
-      <c r="K4" s="6">
-        <v>0</v>
-      </c>
-      <c r="L4" t="s">
-        <v>293</v>
-      </c>
-      <c r="M4" s="6">
-        <v>1</v>
-      </c>
-      <c r="N4" s="6">
+      <c r="K4" s="7">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="M4" s="7">
+        <v>1</v>
+      </c>
+      <c r="N4" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="B5" s="6">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="A5" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
         <v>18.648700000000002</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="7">
         <v>8344</v>
       </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
         <v>562</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="7">
         <v>19</v>
       </c>
-      <c r="K5" s="6">
-        <v>0</v>
-      </c>
-      <c r="L5" t="s">
-        <v>293</v>
-      </c>
-      <c r="M5" s="6">
-        <v>1</v>
-      </c>
-      <c r="N5" s="6">
+      <c r="K5" s="7">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="M5" s="7">
+        <v>1</v>
+      </c>
+      <c r="N5" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6">
+      <c r="A6" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
         <v>31.479500000000002</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="7">
         <v>1490</v>
       </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="6">
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
         <v>774</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="7">
         <v>31</v>
       </c>
-      <c r="K6" s="6">
-        <v>0</v>
-      </c>
-      <c r="L6" t="s">
-        <v>293</v>
-      </c>
-      <c r="M6" s="6">
-        <v>1</v>
-      </c>
-      <c r="N6" s="6">
+      <c r="K6" s="7">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="M6" s="7">
+        <v>1</v>
+      </c>
+      <c r="N6" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="B7" s="6">
-        <v>0</v>
-      </c>
-      <c r="C7" s="6">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6">
+      <c r="A7" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
         <v>49.602899999999998</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="7">
         <v>76830</v>
       </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6">
-        <v>0</v>
-      </c>
-      <c r="I7" s="6">
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7">
         <v>2719</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="7">
         <v>50</v>
       </c>
-      <c r="K7" s="6">
-        <v>0</v>
-      </c>
-      <c r="L7" t="s">
-        <v>293</v>
-      </c>
-      <c r="M7" s="6">
-        <v>1</v>
-      </c>
-      <c r="N7" s="6">
+      <c r="K7" s="7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="M7" s="7">
+        <v>1</v>
+      </c>
+      <c r="N7" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="B8" s="6">
-        <v>0</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6">
+      <c r="A8" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
         <v>1.4E-5</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="7">
         <v>31.479500000000002</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="7">
         <v>99999</v>
       </c>
-      <c r="G8" s="6">
-        <v>0</v>
-      </c>
-      <c r="H8" s="6">
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
         <v>0.31030000000000002</v>
       </c>
-      <c r="I8" s="6">
-        <v>0</v>
-      </c>
-      <c r="J8" s="6">
-        <v>0</v>
-      </c>
-      <c r="K8" s="6">
+      <c r="I8" s="7">
+        <v>0</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
         <v>18084</v>
       </c>
-      <c r="L8" t="s">
-        <v>293</v>
-      </c>
-      <c r="M8" s="6">
-        <v>1</v>
-      </c>
-      <c r="N8" s="6">
+      <c r="L8" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="M8" s="7">
+        <v>1</v>
+      </c>
+      <c r="N8" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="B9" s="6">
-        <v>1</v>
-      </c>
-      <c r="C9" s="6">
-        <v>0</v>
-      </c>
-      <c r="D9" s="6">
+      <c r="A9" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="E9" s="6">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6">
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
         <v>9999</v>
       </c>
-      <c r="G9" s="6">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6">
+      <c r="G9" s="7">
+        <v>0</v>
+      </c>
+      <c r="H9" s="7">
         <v>8.7723999999999996E-2</v>
       </c>
-      <c r="I9" s="6">
-        <v>0</v>
-      </c>
-      <c r="J9" s="6">
-        <v>0</v>
-      </c>
-      <c r="K9" s="6">
+      <c r="I9" s="7">
+        <v>0</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0</v>
+      </c>
+      <c r="K9" s="7">
         <v>0.62702500000000005</v>
       </c>
-      <c r="L9" t="s">
-        <v>293</v>
-      </c>
-      <c r="M9" s="6">
-        <v>1</v>
-      </c>
-      <c r="N9" s="6">
+      <c r="L9" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="M9" s="7">
+        <v>1</v>
+      </c>
+      <c r="N9" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="B10" s="6">
-        <v>0</v>
-      </c>
-      <c r="C10" s="6">
-        <v>1</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0</v>
-      </c>
-      <c r="E10" s="6">
+      <c r="A10" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
         <v>57.408200000000001</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="7">
         <v>410770</v>
       </c>
-      <c r="G10" s="6">
-        <v>0</v>
-      </c>
-      <c r="H10" s="6">
-        <v>0</v>
-      </c>
-      <c r="I10" s="6">
+      <c r="G10" s="7">
+        <v>0</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7">
         <v>5046</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="7">
         <v>57</v>
       </c>
-      <c r="K10" s="6">
-        <v>0</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="K10" s="7">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="M10" s="7">
+        <v>1</v>
+      </c>
+      <c r="N10" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>23.674199999999999</v>
+      </c>
+      <c r="F11" s="7">
+        <v>26112</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7">
+        <v>611</v>
+      </c>
+      <c r="J11" s="7">
+        <v>24</v>
+      </c>
+      <c r="K11" s="7">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="M11" s="7">
+        <v>1</v>
+      </c>
+      <c r="N11" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7">
+        <v>39.284799999999997</v>
+      </c>
+      <c r="F12" s="7">
+        <v>8220</v>
+      </c>
+      <c r="G12" s="7">
+        <v>0</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7">
+        <v>1174</v>
+      </c>
+      <c r="J12" s="7">
+        <v>39</v>
+      </c>
+      <c r="K12" s="7">
+        <v>0</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="M12" s="7">
+        <v>1</v>
+      </c>
+      <c r="N12" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>18.648700000000002</v>
+      </c>
+      <c r="F13" s="7">
+        <v>8344</v>
+      </c>
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7">
+        <v>562</v>
+      </c>
+      <c r="J13" s="7">
+        <v>19</v>
+      </c>
+      <c r="K13" s="7">
+        <v>0</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="M13" s="7">
+        <v>1</v>
+      </c>
+      <c r="N13" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="B14" s="7">
+        <v>0</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7">
+        <v>31.479500000000002</v>
+      </c>
+      <c r="F14" s="7">
+        <v>1490</v>
+      </c>
+      <c r="G14" s="7">
+        <v>0</v>
+      </c>
+      <c r="H14" s="7">
+        <v>0</v>
+      </c>
+      <c r="I14" s="7">
+        <v>774</v>
+      </c>
+      <c r="J14" s="7">
+        <v>31</v>
+      </c>
+      <c r="K14" s="7">
+        <v>0</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="M14" s="7">
+        <v>1</v>
+      </c>
+      <c r="N14" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="B15" s="7">
+        <v>0</v>
+      </c>
+      <c r="C15" s="7">
+        <v>1</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7">
+        <v>49.602899999999998</v>
+      </c>
+      <c r="F15" s="7">
+        <v>76830</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0</v>
+      </c>
+      <c r="H15" s="7">
+        <v>0</v>
+      </c>
+      <c r="I15" s="7">
+        <v>2719</v>
+      </c>
+      <c r="J15" s="7">
+        <v>50</v>
+      </c>
+      <c r="K15" s="7">
+        <v>0</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="M15" s="7">
+        <v>1</v>
+      </c>
+      <c r="N15" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="M10" s="6">
-        <v>1</v>
-      </c>
-      <c r="N10" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="B11" s="6">
-        <v>0</v>
-      </c>
-      <c r="C11" s="6">
-        <v>1</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6">
-        <v>23.674199999999999</v>
-      </c>
-      <c r="F11" s="6">
-        <v>26112</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0</v>
-      </c>
-      <c r="H11" s="6">
-        <v>0</v>
-      </c>
-      <c r="I11" s="6">
-        <v>611</v>
-      </c>
-      <c r="J11" s="6">
-        <v>24</v>
-      </c>
-      <c r="K11" s="6">
-        <v>0</v>
-      </c>
-      <c r="L11" t="s">
-        <v>302</v>
-      </c>
-      <c r="M11" s="6">
-        <v>1</v>
-      </c>
-      <c r="N11" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="B12" s="6">
-        <v>0</v>
-      </c>
-      <c r="C12" s="6">
-        <v>1</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6">
-        <v>39.284799999999997</v>
-      </c>
-      <c r="F12" s="6">
-        <v>8220</v>
-      </c>
-      <c r="G12" s="6">
-        <v>0</v>
-      </c>
-      <c r="H12" s="6">
-        <v>0</v>
-      </c>
-      <c r="I12" s="6">
-        <v>1174</v>
-      </c>
-      <c r="J12" s="6">
-        <v>39</v>
-      </c>
-      <c r="K12" s="6">
-        <v>0</v>
-      </c>
-      <c r="L12" t="s">
-        <v>302</v>
-      </c>
-      <c r="M12" s="6">
-        <v>1</v>
-      </c>
-      <c r="N12" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="B13" s="6">
-        <v>0</v>
-      </c>
-      <c r="C13" s="6">
-        <v>1</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0</v>
-      </c>
-      <c r="E13" s="6">
-        <v>18.648700000000002</v>
-      </c>
-      <c r="F13" s="6">
-        <v>8344</v>
-      </c>
-      <c r="G13" s="6">
-        <v>0</v>
-      </c>
-      <c r="H13" s="6">
-        <v>0</v>
-      </c>
-      <c r="I13" s="6">
-        <v>562</v>
-      </c>
-      <c r="J13" s="6">
-        <v>19</v>
-      </c>
-      <c r="K13" s="6">
-        <v>0</v>
-      </c>
-      <c r="L13" t="s">
-        <v>302</v>
-      </c>
-      <c r="M13" s="6">
-        <v>1</v>
-      </c>
-      <c r="N13" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="B14" s="6">
-        <v>0</v>
-      </c>
-      <c r="C14" s="6">
-        <v>1</v>
-      </c>
-      <c r="D14" s="6">
-        <v>0</v>
-      </c>
-      <c r="E14" s="6">
+      <c r="B16" s="7">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1.4E-5</v>
+      </c>
+      <c r="E16" s="7">
         <v>31.479500000000002</v>
       </c>
-      <c r="F14" s="6">
-        <v>1490</v>
-      </c>
-      <c r="G14" s="6">
-        <v>0</v>
-      </c>
-      <c r="H14" s="6">
-        <v>0</v>
-      </c>
-      <c r="I14" s="6">
-        <v>774</v>
-      </c>
-      <c r="J14" s="6">
-        <v>31</v>
-      </c>
-      <c r="K14" s="6">
-        <v>0</v>
-      </c>
-      <c r="L14" t="s">
-        <v>302</v>
-      </c>
-      <c r="M14" s="6">
-        <v>1</v>
-      </c>
-      <c r="N14" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="B15" s="6">
-        <v>0</v>
-      </c>
-      <c r="C15" s="6">
-        <v>1</v>
-      </c>
-      <c r="D15" s="6">
-        <v>0</v>
-      </c>
-      <c r="E15" s="6">
-        <v>49.602899999999998</v>
-      </c>
-      <c r="F15" s="6">
-        <v>76830</v>
-      </c>
-      <c r="G15" s="6">
-        <v>0</v>
-      </c>
-      <c r="H15" s="6">
-        <v>0</v>
-      </c>
-      <c r="I15" s="6">
-        <v>2719</v>
-      </c>
-      <c r="J15" s="6">
-        <v>50</v>
-      </c>
-      <c r="K15" s="6">
-        <v>0</v>
-      </c>
-      <c r="L15" t="s">
-        <v>302</v>
-      </c>
-      <c r="M15" s="6">
-        <v>1</v>
-      </c>
-      <c r="N15" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="B16" s="6">
-        <v>0</v>
-      </c>
-      <c r="C16" s="6">
-        <v>0</v>
-      </c>
-      <c r="D16" s="6">
-        <v>1.4E-5</v>
-      </c>
-      <c r="E16" s="6">
-        <v>31.479500000000002</v>
-      </c>
-      <c r="F16" s="6">
+      <c r="F16" s="7">
         <v>99999</v>
       </c>
-      <c r="G16" s="6">
-        <v>0</v>
-      </c>
-      <c r="H16" s="6">
+      <c r="G16" s="7">
+        <v>0</v>
+      </c>
+      <c r="H16" s="7">
         <v>0.31030000000000002</v>
       </c>
-      <c r="I16" s="6">
-        <v>0</v>
-      </c>
-      <c r="J16" s="6">
-        <v>0</v>
-      </c>
-      <c r="K16" s="6">
+      <c r="I16" s="7">
+        <v>0</v>
+      </c>
+      <c r="J16" s="7">
+        <v>0</v>
+      </c>
+      <c r="K16" s="7">
         <v>18084</v>
       </c>
-      <c r="L16" t="s">
-        <v>302</v>
-      </c>
-      <c r="M16" s="6">
-        <v>1</v>
-      </c>
-      <c r="N16" s="6">
+      <c r="L16" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="M16" s="7">
+        <v>1</v>
+      </c>
+      <c r="N16" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="B17" s="6">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6">
-        <v>0</v>
-      </c>
-      <c r="D17" s="6">
+      <c r="A17" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="B17" s="7">
+        <v>1</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0</v>
+      </c>
+      <c r="D17" s="7">
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="E17" s="6">
-        <v>0</v>
-      </c>
-      <c r="F17" s="6">
+      <c r="E17" s="7">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7">
         <v>9999</v>
       </c>
-      <c r="G17" s="6">
-        <v>0</v>
-      </c>
-      <c r="H17" s="6">
+      <c r="G17" s="7">
+        <v>0</v>
+      </c>
+      <c r="H17" s="7">
         <v>8.7723999999999996E-2</v>
       </c>
-      <c r="I17" s="6">
-        <v>0</v>
-      </c>
-      <c r="J17" s="6">
-        <v>0</v>
-      </c>
-      <c r="K17" s="6">
+      <c r="I17" s="7">
+        <v>0</v>
+      </c>
+      <c r="J17" s="7">
+        <v>0</v>
+      </c>
+      <c r="K17" s="7">
         <v>0.62702500000000005</v>
       </c>
-      <c r="L17" t="s">
-        <v>302</v>
-      </c>
-      <c r="M17" s="6">
-        <v>1</v>
-      </c>
-      <c r="N17" s="6">
+      <c r="L17" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="M17" s="7">
+        <v>1</v>
+      </c>
+      <c r="N17" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3961,11 +3964,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F3139F5-D92A-014A-995D-4369696ABFF0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50C7D64-4057-8943-93B3-6C3E32E119D3}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3979,82 +3982,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="A1" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="B2" s="6">
+      <c r="A2" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" s="7">
         <v>0.15655827580000001</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <v>0.91229020000000005</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="7">
         <v>2.898939E-2</v>
       </c>
-      <c r="E2" s="6">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6">
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="B3" s="6">
+      <c r="A3" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="B3" s="7">
         <v>85</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="8">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="7">
         <v>0.98</v>
       </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6">
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>301</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
+      <c r="A4" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4067,8 +4070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6075F4E-6449-42F6-B0A2-E3B463F49D3C}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4172,7 +4175,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -4195,7 +4198,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>275</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4210,7 +4213,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>6.2899999999999998E-2</v>
+        <v>6.8699999999999997E-2</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -4224,7 +4227,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>276</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4253,25 +4256,25 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>277</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>-6.83E-2</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>2.53E-2</v>
       </c>
       <c r="G8">
-        <v>-27</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -4282,7 +4285,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -4297,13 +4300,13 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.22</v>
+        <v>6.2899999999999998E-2</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>366</v>
+        <v>0</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -4311,7 +4314,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -4326,7 +4329,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>2.53E-2</v>
+        <v>4.5199999999999997E-2</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -4340,25 +4343,25 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>-6.83E-2</v>
       </c>
       <c r="F11">
-        <v>9.7000000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>-27</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -4369,28 +4372,28 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>-6.8199999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.22</v>
       </c>
       <c r="G12">
-        <v>-308</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>366</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -4398,25 +4401,25 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>-0.128</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>2.53E-2</v>
       </c>
       <c r="G13">
-        <v>-130</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -4427,7 +4430,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -4442,13 +4445,13 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>0.16539999999999999</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>366</v>
+        <v>0</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -4456,28 +4459,28 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>-6.8199999999999997E-2</v>
       </c>
       <c r="F15">
-        <v>0.16539999999999999</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>-308</v>
       </c>
       <c r="H15">
-        <v>366</v>
+        <v>0</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -4485,25 +4488,25 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>-0.128</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>-130</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -4514,7 +4517,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -4523,19 +4526,19 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
-        <v>1.4999999999999999E-2</v>
+        <v>0.16539999999999999</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>436</v>
+        <v>366</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -4543,28 +4546,28 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>0.16539999999999999</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>366</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -4572,7 +4575,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -4581,19 +4584,19 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>0.15620000000000001</v>
+        <v>0</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -4601,7 +4604,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -4616,13 +4619,13 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>436</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -4630,28 +4633,28 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
-        <v>0.16539999999999999</v>
+        <v>0</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
-        <v>366</v>
+        <v>0</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -4659,7 +4662,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -4674,13 +4677,13 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>2.53E-2</v>
+        <v>0.15620000000000001</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -4688,25 +4691,25 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>-5.1459999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23">
-        <v>-27</v>
+        <v>0</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -4717,7 +4720,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -4732,13 +4735,13 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>9.4500000000000001E-2</v>
+        <v>0.16539999999999999</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>366</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -4746,25 +4749,25 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>-0.128</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>2.53E-2</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -4775,28 +4778,28 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>-5.1459999999999999E-2</v>
       </c>
       <c r="F26">
-        <v>2.9000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>-27</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -4804,28 +4807,28 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>-0.128</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>9.4500000000000001E-2</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -4833,25 +4836,25 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>-0.128</v>
       </c>
       <c r="F28">
-        <v>2.53E-2</v>
+        <v>0</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -4862,7 +4865,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -4877,13 +4880,13 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>9.7000000000000003E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="G29">
         <v>0</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -4891,25 +4894,25 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>-0.128</v>
       </c>
       <c r="F30">
-        <v>9.4500000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -4920,7 +4923,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -4935,7 +4938,7 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>2.9000000000000001E-2</v>
+        <v>2.53E-2</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -4949,7 +4952,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>307</v>
+        <v>46</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -4964,7 +4967,7 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>6.2899999999999998E-2</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -4978,7 +4981,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>308</v>
+        <v>47</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -4993,7 +4996,7 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>4.5199999999999997E-2</v>
+        <v>9.4500000000000001E-2</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -5007,7 +5010,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>309</v>
+        <v>48</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -5022,7 +5025,7 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <v>2.53E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -5035,13 +5038,18 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:I32">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+  <conditionalFormatting sqref="B3:I5 B9:I34 F6">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B33:I34">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="B6:I6">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:I8">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5055,7 +5063,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5098,7 +5106,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>278</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5127,7 +5135,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>304</v>
+        <v>279</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5156,7 +5164,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>305</v>
+        <v>280</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -5185,7 +5193,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>306</v>
+        <v>281</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5852,7 +5860,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:I28">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13944,7 +13952,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:X110">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14156,7 +14164,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:U3">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14773,12 +14781,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:AF5">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:AF7">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14791,7 +14799,7 @@
   <dimension ref="A1:AQ24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17684,7 +17692,7 @@
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>310</v>
+        <v>274</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -17711,7 +17719,7 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>232</v>
+        <v>317</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -17726,7 +17734,7 @@
         <v>999</v>
       </c>
       <c r="O24">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="P24">
         <v>1.0000000000000001E-5</v>
@@ -17814,13 +17822,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:AQ23">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24:AQ24">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="B3:AQ24">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18424,7 +18427,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:AA8">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18914,7 +18917,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:O11">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
input(standart_parameters.xlsx): added fuel cell heat bus
</commit_message>
<xml_diff>
--- a/program_files/urban_district_upscaling/standard_parameters.xlsx
+++ b/program_files/urban_district_upscaling/standard_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SESMG-dev\SESMG-dev\program_files\urban_district_upscaling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klemm\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A902303-892E-4DAE-B2E9-50F7D7E18596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DF2C6E-F663-4078-81CE-477B57C2A97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="5" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="1" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
   <sheets>
     <sheet name="energysystem" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="8_pipe_types" sheetId="12" r:id="rId11"/>
     <sheet name="8_1_other" sheetId="13" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="335">
   <si>
     <t>start date</t>
   </si>
@@ -1049,6 +1049,9 @@
   </si>
   <si>
     <t>cluster_electricity_link</t>
+  </si>
+  <si>
+    <t>central_fc_heat_bus</t>
   </si>
 </sst>
 </file>
@@ -4689,10 +4692,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6075F4E-6449-42F6-B0A2-E3B463F49D3C}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5090,7 +5093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -5116,7 +5119,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -5142,7 +5145,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -5168,7 +5171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -5194,7 +5197,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -5220,7 +5223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -5246,261 +5249,264 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>334</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>39</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>40</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
         <v>0.1958</v>
       </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
         <v>366</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>41</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>322</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
         <v>-0.1215</v>
       </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
         <v>-1.39</v>
       </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="H27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>42</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
         <v>-5.1459999999999999E-2</v>
       </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
         <v>-27</v>
       </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>43</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
         <v>9.4500000000000001E-2</v>
       </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>44</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
         <v>-0.128</v>
       </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
         <v>-95</v>
       </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="H30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>45</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>46</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
         <v>-0.128</v>
       </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
         <v>-95</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -5508,7 +5514,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -5523,7 +5529,7 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>9.7000000000000003E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -5534,7 +5540,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -5549,7 +5555,7 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <v>9.4500000000000001E-2</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -5560,32 +5566,58 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>9.4500000000000001E-2</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>50</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:H5 F6 B9:H14 B17:H35 B15:F16 H15:H16">
+  <conditionalFormatting sqref="B3:H5 F6 B9:H14 B15:F16 H15:H16 B17:H22 B24:H36">
     <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -15620,7 +15652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865B2AF4-2CF4-4093-8D70-C931333F20A4}">
   <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="AF3" sqref="AF3:AG7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
input_files(standard_parameters.xlsx): added h2_heat_bus and h2_heat_link
</commit_message>
<xml_diff>
--- a/program_files/urban_district_upscaling/standard_parameters.xlsx
+++ b/program_files/urban_district_upscaling/standard_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klemm\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DF2C6E-F663-4078-81CE-477B57C2A97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F2CF23-8875-4301-97E3-05D3838FD31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="1" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
+    <workbookView xWindow="-16320" yWindow="-30" windowWidth="16440" windowHeight="28320" firstSheet="4" activeTab="8" xr2:uid="{D48BE4BC-BA48-4DC0-B3DF-D04B8CFD99C7}"/>
   </bookViews>
   <sheets>
     <sheet name="energysystem" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="8_pipe_types" sheetId="12" r:id="rId11"/>
     <sheet name="8_1_other" sheetId="13" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="336">
   <si>
     <t>start date</t>
   </si>
@@ -1051,7 +1051,10 @@
     <t>cluster_electricity_link</t>
   </si>
   <si>
-    <t>central_fc_heat_bus</t>
+    <t>central_h2_heat_link</t>
+  </si>
+  <si>
+    <t>central_h2_heat_bus</t>
   </si>
 </sst>
 </file>
@@ -1231,7 +1234,14 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 3" xfId="1" xr:uid="{3EB3DAA0-9F71-48CB-8FEA-1E1CAF40E04C}"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3351,7 +3361,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:D116">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4573,12 +4583,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J7">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4694,7 +4704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6075F4E-6449-42F6-B0A2-E3B463F49D3C}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -5251,7 +5261,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -5618,22 +5628,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:H5 F6 B9:H14 B15:F16 H15:H16 B17:H22 B24:H36">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:H6">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:H8">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:G16">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6589,7 +6599,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:I26 B31:I32">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15410,7 +15420,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:Z110">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15640,7 +15650,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:W3">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16276,7 +16286,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:AG7">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16288,8 +16298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFB4EA7-D669-4B1E-9B4E-C2CB3560F5F3}">
   <dimension ref="A1:AP24"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17200,7 +17210,7 @@
         <v>233</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
         <v>226</v>
@@ -19245,7 +19255,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:AP24">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19849,7 +19859,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:AA8">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19859,10 +19869,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F7A117-64AB-4955-A232-50A2E399D809}">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20662,14 +20672,63 @@
         <v>0</v>
       </c>
     </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>334</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>271</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>9999</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K20">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:N18">
+  <conditionalFormatting sqref="A3:N18 A20:C20">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:N19">
     <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19:N19">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="D20:N20">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>